<commit_message>
adaptive, smart final, N150
</commit_message>
<xml_diff>
--- a/results/DR_batches_summary.xlsx
+++ b/results/DR_batches_summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8607d062d2dc3d62/EV-projects/evcs-projects/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_23F921EDCB5B0B12912D4CEA75A631074FBA864A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{935A5AAC-7BA5-43BD-A7FF-4ADB229AB09D}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_23F921EDCB5B0B12912D4CEA75A631074FBA864A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{442283A7-59BE-4DF8-96C8-A5CF3078A395}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="24792" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,9 +189,7 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -210,7 +208,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -221,6 +263,56 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1433B753-A71F-44FC-96D2-AC8CE580C67C}" name="Table1" displayName="Table1" ref="A1:AO11" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:AO11" xr:uid="{1433B753-A71F-44FC-96D2-AC8CE580C67C}"/>
+  <tableColumns count="41">
+    <tableColumn id="1" xr3:uid="{4AC64729-C96F-495C-8694-E8DC3D93C30D}" name="iter_from"/>
+    <tableColumn id="2" xr3:uid="{DF6C84BB-E9FF-4E5D-AA34-C9BE02690AD0}" name="iter_to"/>
+    <tableColumn id="3" xr3:uid="{961BF1E6-1CFB-44E7-8D36-2B8903E32C4D}" name="best_start"/>
+    <tableColumn id="4" xr3:uid="{A7F70EC4-1F51-4FEF-BC0A-A58C30C3806D}" name="best_end"/>
+    <tableColumn id="5" xr3:uid="{0ED88D78-5956-4544-953B-EC6C5CE97190}" name="batch_best_improvement"/>
+    <tableColumn id="6" xr3:uid="{2F8EAF82-DEE8-4E08-AAD5-11EFF96168F6}" name="site_all_picked"/>
+    <tableColumn id="7" xr3:uid="{92414B0A-090A-434B-8221-807F54D80C0E}" name="site_all_accepted"/>
+    <tableColumn id="8" xr3:uid="{42391D3A-6091-4E4B-A4AE-30A8547434EE}" name="site_all_acc_rate"/>
+    <tableColumn id="9" xr3:uid="{FEE9CB0E-B356-4980-AEC7-010DCEF7BCF9}" name="site_all_impr_curr"/>
+    <tableColumn id="10" xr3:uid="{A530247C-6A0C-48DB-92BC-5910F20EED63}" name="site_all_impr_best"/>
+    <tableColumn id="11" xr3:uid="{E310961B-2455-49E4-83FE-9F11D30B0D59}" name="site_all_best_delta"/>
+    <tableColumn id="12" xr3:uid="{6E0D4DFA-F890-4231-BDFD-F0920F59F37C}" name="site_all_reward_sum"/>
+    <tableColumn id="13" xr3:uid="{9A41519C-380F-4FFA-BDDC-4BB164519DA6}" name="site_all_avg_reward"/>
+    <tableColumn id="14" xr3:uid="{14E3A4BF-AC9D-4A09-A9A6-55A3272EAB78}" name="p_site_all"/>
+    <tableColumn id="15" xr3:uid="{F9D868B6-D152-42AF-995B-1F18E337EB8E}" name="site_future_picked"/>
+    <tableColumn id="16" xr3:uid="{800841D3-FA33-4808-834F-8147A70ABCD0}" name="site_future_accepted"/>
+    <tableColumn id="17" xr3:uid="{A8D0EA32-FBE8-4C32-8D33-D41BAA2CFD41}" name="site_future_acc_rate"/>
+    <tableColumn id="18" xr3:uid="{BDB45661-1710-45C9-B2BB-D6291A104F35}" name="site_future_impr_curr"/>
+    <tableColumn id="19" xr3:uid="{039FCE16-60C5-40D3-BF13-3542D0826AFA}" name="site_future_impr_best"/>
+    <tableColumn id="20" xr3:uid="{CEC15455-9D89-465E-A88E-A76E65D42E5A}" name="site_future_best_delta"/>
+    <tableColumn id="21" xr3:uid="{B2C01EA0-1D9B-4D04-876E-85C753F2B08C}" name="site_future_reward_sum"/>
+    <tableColumn id="22" xr3:uid="{46A98BF5-4EA4-403F-B10F-F37BBBE576DB}" name="site_future_avg_reward"/>
+    <tableColumn id="23" xr3:uid="{3EF45CD5-DE7C-45FD-A52E-52C8BEC2AB37}" name="p_site_future"/>
+    <tableColumn id="24" xr3:uid="{BEC64B59-A43E-424C-927C-992607591B80}" name="site_swap_picked"/>
+    <tableColumn id="25" xr3:uid="{60F7C455-321A-4563-8D6F-6FDD742D7AFA}" name="site_swap_accepted"/>
+    <tableColumn id="26" xr3:uid="{8383EB91-CD99-43A2-9072-00DBA9514CC4}" name="site_swap_acc_rate"/>
+    <tableColumn id="27" xr3:uid="{3794F587-FA08-4238-B4EA-2C25A8499675}" name="site_swap_impr_curr"/>
+    <tableColumn id="28" xr3:uid="{F87E6AD1-C480-4120-9B34-598E7F6197A0}" name="site_swap_impr_best"/>
+    <tableColumn id="29" xr3:uid="{1CFB4315-A5E9-4A2B-BB6F-44DCB104BF6D}" name="site_swap_best_delta"/>
+    <tableColumn id="30" xr3:uid="{3DB19318-F301-4311-B9AA-B59899117D61}" name="site_swap_reward_sum"/>
+    <tableColumn id="31" xr3:uid="{0227EBCC-0D2E-46D8-B74F-046766CA165A}" name="site_swap_avg_reward"/>
+    <tableColumn id="32" xr3:uid="{B91BB01B-798E-48E4-9B0B-D72D2DD94EE7}" name="p_site_swap"/>
+    <tableColumn id="33" xr3:uid="{7529F0A6-7A93-41A3-BC1A-9AC221F07F02}" name="k_units_picked"/>
+    <tableColumn id="34" xr3:uid="{39093A2A-087B-48FC-AFF8-B1935E9BB65F}" name="k_units_accepted"/>
+    <tableColumn id="35" xr3:uid="{38B218BD-3A0A-46D0-8960-C9F869FAA017}" name="k_units_acc_rate"/>
+    <tableColumn id="36" xr3:uid="{9656E147-630D-4780-B978-E278FE76D8D6}" name="k_units_impr_curr"/>
+    <tableColumn id="37" xr3:uid="{DD2537EA-764C-430E-BFEC-CC6D06D4B1BF}" name="k_units_impr_best"/>
+    <tableColumn id="38" xr3:uid="{497DFE05-EFE1-42FD-B270-6A864A723405}" name="k_units_best_delta"/>
+    <tableColumn id="39" xr3:uid="{E4168486-9143-4FE6-9659-8631B12DC1E6}" name="k_units_reward_sum"/>
+    <tableColumn id="40" xr3:uid="{3CF72DF9-7DEE-486A-8464-49A9EB2DEB46}" name="k_units_avg_reward"/>
+    <tableColumn id="41" xr3:uid="{773B875C-FC1E-4BA8-85DE-8EECE3A96D2D}" name="p_k_units"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -512,20 +604,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" customWidth="1"/>
+    <col min="12" max="12" width="20.109375" customWidth="1"/>
+    <col min="13" max="13" width="19.5546875" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="18.5546875" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" customWidth="1"/>
+    <col min="17" max="17" width="20.109375" customWidth="1"/>
+    <col min="18" max="18" width="21.21875" customWidth="1"/>
+    <col min="19" max="19" width="21.44140625" customWidth="1"/>
+    <col min="20" max="20" width="21.77734375" customWidth="1"/>
+    <col min="21" max="21" width="23.44140625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="22.88671875" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="16.6640625" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="19.77734375" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="19.21875" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="20.33203125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="23.33203125" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25.33203125" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="22" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="15.77734375" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="15.5546875" customWidth="1"/>
+    <col min="34" max="34" width="17.6640625" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="17.109375" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="18.21875" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="18.44140625" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.44140625" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="19.88671875" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="11.109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.3">
@@ -1905,5 +2029,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>